<commit_message>
Fix analysis accuracy and enhance visualizations
</commit_message>
<xml_diff>
--- a/Data/Cleaned_Merged_Dataset.xlsx
+++ b/Data/Cleaned_Merged_Dataset.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Z17"/>
+  <dimension ref="A1:X17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -455,12 +455,12 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Meal Type_x</t>
+          <t>Meal Type</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Dish Name_x</t>
+          <t>Dish Name</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
@@ -490,80 +490,70 @@
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>Dish Name_y</t>
+          <t>Session Start</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>Meal Type_y</t>
+          <t>Session End</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>Session Start</t>
+          <t>Duration (mins)</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>Session End</t>
+          <t>Session Rating</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>Duration (mins)</t>
+          <t>User Name</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>Session Rating</t>
+          <t>Age</t>
         </is>
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>User Name</t>
+          <t>Location</t>
         </is>
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
-          <t>Age</t>
+          <t>Registration Date</t>
         </is>
       </c>
       <c r="S1" s="1" t="inlineStr">
         <is>
-          <t>Location</t>
+          <t>Phone</t>
         </is>
       </c>
       <c r="T1" s="1" t="inlineStr">
         <is>
-          <t>Registration Date</t>
+          <t>Email</t>
         </is>
       </c>
       <c r="U1" s="1" t="inlineStr">
         <is>
-          <t>Phone</t>
+          <t>Favorite Meal</t>
         </is>
       </c>
       <c r="V1" s="1" t="inlineStr">
         <is>
-          <t>Email</t>
+          <t>Total Orders</t>
         </is>
       </c>
       <c r="W1" s="1" t="inlineStr">
         <is>
-          <t>Favorite Meal</t>
+          <t>Order Amount per Minute</t>
         </is>
       </c>
       <c r="X1" s="1" t="inlineStr">
-        <is>
-          <t>Total Orders</t>
-        </is>
-      </c>
-      <c r="Y1" s="1" t="inlineStr">
-        <is>
-          <t>Order Amount per Minute</t>
-        </is>
-      </c>
-      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>Is Canceled</t>
         </is>
@@ -612,66 +602,56 @@
           <t>S001</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>Spaghetti</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
+      <c r="K2" s="2" t="n">
+        <v>45627.79166666666</v>
+      </c>
+      <c r="L2" s="2" t="n">
+        <v>45627.8125</v>
+      </c>
+      <c r="M2" t="n">
+        <v>30</v>
+      </c>
+      <c r="N2" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>Alice Johnson</t>
+        </is>
+      </c>
+      <c r="P2" t="n">
+        <v>28</v>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>New York</t>
+        </is>
+      </c>
+      <c r="R2" s="2" t="n">
+        <v>44941</v>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>123-456-7890</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>alice@email.com</t>
+        </is>
+      </c>
+      <c r="U2" t="inlineStr">
         <is>
           <t>Dinner</t>
         </is>
       </c>
-      <c r="M2" s="2" t="n">
-        <v>45627.79166666666</v>
-      </c>
-      <c r="N2" s="2" t="n">
-        <v>45627.8125</v>
-      </c>
-      <c r="O2" t="n">
-        <v>30</v>
-      </c>
-      <c r="P2" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="Q2" t="inlineStr">
-        <is>
-          <t>Alice Johnson</t>
-        </is>
-      </c>
-      <c r="R2" t="n">
-        <v>28</v>
-      </c>
-      <c r="S2" t="inlineStr">
-        <is>
-          <t>New York</t>
-        </is>
-      </c>
-      <c r="T2" s="2" t="n">
-        <v>44941</v>
-      </c>
-      <c r="U2" t="inlineStr">
-        <is>
-          <t>123-456-7890</t>
-        </is>
-      </c>
-      <c r="V2" t="inlineStr">
-        <is>
-          <t>alice@email.com</t>
-        </is>
-      </c>
-      <c r="W2" t="inlineStr">
-        <is>
-          <t>Dinner</t>
-        </is>
+      <c r="V2" t="n">
+        <v>12</v>
+      </c>
+      <c r="W2" t="n">
+        <v>0.5</v>
       </c>
       <c r="X2" t="n">
-        <v>12</v>
-      </c>
-      <c r="Y2" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="Z2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -718,66 +698,56 @@
           <t>S002</t>
         </is>
       </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>Caesar Salad</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
+      <c r="K3" s="2" t="n">
+        <v>45627.5</v>
+      </c>
+      <c r="L3" s="2" t="n">
+        <v>45627.51388888889</v>
+      </c>
+      <c r="M3" t="n">
+        <v>20</v>
+      </c>
+      <c r="N3" t="n">
+        <v>4</v>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>Bob Smith</t>
+        </is>
+      </c>
+      <c r="P3" t="n">
+        <v>35</v>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>Los Angeles</t>
+        </is>
+      </c>
+      <c r="R3" s="2" t="n">
+        <v>44977</v>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>987-654-3210</t>
+        </is>
+      </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>bob@email.com</t>
+        </is>
+      </c>
+      <c r="U3" t="inlineStr">
         <is>
           <t>Lunch</t>
         </is>
       </c>
-      <c r="M3" s="2" t="n">
-        <v>45627.5</v>
-      </c>
-      <c r="N3" s="2" t="n">
-        <v>45627.51388888889</v>
-      </c>
-      <c r="O3" t="n">
-        <v>20</v>
-      </c>
-      <c r="P3" t="n">
-        <v>4</v>
-      </c>
-      <c r="Q3" t="inlineStr">
-        <is>
-          <t>Bob Smith</t>
-        </is>
-      </c>
-      <c r="R3" t="n">
-        <v>35</v>
-      </c>
-      <c r="S3" t="inlineStr">
-        <is>
-          <t>Los Angeles</t>
-        </is>
-      </c>
-      <c r="T3" s="2" t="n">
-        <v>44977</v>
-      </c>
-      <c r="U3" t="inlineStr">
-        <is>
-          <t>987-654-3210</t>
-        </is>
-      </c>
-      <c r="V3" t="inlineStr">
-        <is>
-          <t>bob@email.com</t>
-        </is>
-      </c>
-      <c r="W3" t="inlineStr">
-        <is>
-          <t>Lunch</t>
-        </is>
+      <c r="V3" t="n">
+        <v>8</v>
+      </c>
+      <c r="W3" t="n">
+        <v>0.5</v>
       </c>
       <c r="X3" t="n">
-        <v>8</v>
-      </c>
-      <c r="Y3" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="Z3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -824,66 +794,56 @@
           <t>S003</t>
         </is>
       </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>Grilled Chicken</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>Dinner</t>
-        </is>
-      </c>
-      <c r="M4" s="2" t="n">
+      <c r="K4" s="2" t="n">
         <v>45628.8125</v>
       </c>
-      <c r="N4" s="2" t="n">
+      <c r="L4" s="2" t="n">
         <v>45628.84027777778</v>
       </c>
-      <c r="O4" t="n">
+      <c r="M4" t="n">
         <v>40</v>
       </c>
+      <c r="N4" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>Charlie Lee</t>
+        </is>
+      </c>
       <c r="P4" t="n">
-        <v>4.8</v>
+        <v>42</v>
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>Charlie Lee</t>
-        </is>
-      </c>
-      <c r="R4" t="n">
-        <v>42</v>
+          <t>Chicago</t>
+        </is>
+      </c>
+      <c r="R4" s="2" t="n">
+        <v>44995</v>
       </c>
       <c r="S4" t="inlineStr">
         <is>
-          <t>Chicago</t>
-        </is>
-      </c>
-      <c r="T4" s="2" t="n">
-        <v>44995</v>
+          <t>555-123-4567</t>
+        </is>
+      </c>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t>charlie@email.com</t>
+        </is>
       </c>
       <c r="U4" t="inlineStr">
         <is>
-          <t>555-123-4567</t>
-        </is>
-      </c>
-      <c r="V4" t="inlineStr">
-        <is>
-          <t>charlie@email.com</t>
-        </is>
-      </c>
-      <c r="W4" t="inlineStr">
-        <is>
           <t>Breakfast</t>
         </is>
       </c>
+      <c r="V4" t="n">
+        <v>15</v>
+      </c>
+      <c r="W4" t="n">
+        <v>0.3125</v>
+      </c>
       <c r="X4" t="n">
-        <v>15</v>
-      </c>
-      <c r="Y4" t="n">
-        <v>0.3125</v>
-      </c>
-      <c r="Z4" t="n">
         <v>1</v>
       </c>
     </row>
@@ -930,66 +890,56 @@
           <t>S004</t>
         </is>
       </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>Pancakes</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>Breakfast</t>
-        </is>
-      </c>
-      <c r="M5" s="2" t="n">
+      <c r="K5" s="2" t="n">
         <v>45628.3125</v>
       </c>
-      <c r="N5" s="2" t="n">
+      <c r="L5" s="2" t="n">
         <v>45628.33333333334</v>
       </c>
-      <c r="O5" t="n">
+      <c r="M5" t="n">
         <v>30</v>
       </c>
+      <c r="N5" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>Alice Johnson</t>
+        </is>
+      </c>
       <c r="P5" t="n">
-        <v>4.2</v>
+        <v>28</v>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>Alice Johnson</t>
-        </is>
-      </c>
-      <c r="R5" t="n">
-        <v>28</v>
+          <t>New York</t>
+        </is>
+      </c>
+      <c r="R5" s="2" t="n">
+        <v>44941</v>
       </c>
       <c r="S5" t="inlineStr">
         <is>
-          <t>New York</t>
-        </is>
-      </c>
-      <c r="T5" s="2" t="n">
-        <v>44941</v>
+          <t>123-456-7890</t>
+        </is>
+      </c>
+      <c r="T5" t="inlineStr">
+        <is>
+          <t>alice@email.com</t>
+        </is>
       </c>
       <c r="U5" t="inlineStr">
         <is>
-          <t>123-456-7890</t>
-        </is>
-      </c>
-      <c r="V5" t="inlineStr">
-        <is>
-          <t>alice@email.com</t>
-        </is>
-      </c>
-      <c r="W5" t="inlineStr">
-        <is>
           <t>Dinner</t>
         </is>
       </c>
+      <c r="V5" t="n">
+        <v>12</v>
+      </c>
+      <c r="W5" t="n">
+        <v>0.2666666666666667</v>
+      </c>
       <c r="X5" t="n">
-        <v>12</v>
-      </c>
-      <c r="Y5" t="n">
-        <v>0.2666666666666667</v>
-      </c>
-      <c r="Z5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1036,66 +986,56 @@
           <t>S005</t>
         </is>
       </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>Caesar Salad</t>
-        </is>
-      </c>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>Lunch</t>
-        </is>
-      </c>
-      <c r="M6" s="2" t="n">
+      <c r="K6" s="2" t="n">
         <v>45629.54166666666</v>
       </c>
-      <c r="N6" s="2" t="n">
+      <c r="L6" s="2" t="n">
         <v>45629.55208333334</v>
       </c>
-      <c r="O6" t="n">
+      <c r="M6" t="n">
         <v>15</v>
       </c>
+      <c r="N6" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>David Brown</t>
+        </is>
+      </c>
       <c r="P6" t="n">
-        <v>4.7</v>
+        <v>27</v>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>David Brown</t>
-        </is>
-      </c>
-      <c r="R6" t="n">
-        <v>27</v>
+          <t>San Francisco</t>
+        </is>
+      </c>
+      <c r="R6" s="2" t="n">
+        <v>45021</v>
       </c>
       <c r="S6" t="inlineStr">
         <is>
-          <t>San Francisco</t>
-        </is>
-      </c>
-      <c r="T6" s="2" t="n">
-        <v>45021</v>
+          <t>444-333-2222</t>
+        </is>
+      </c>
+      <c r="T6" t="inlineStr">
+        <is>
+          <t>david@email.com</t>
+        </is>
       </c>
       <c r="U6" t="inlineStr">
         <is>
-          <t>444-333-2222</t>
-        </is>
-      </c>
-      <c r="V6" t="inlineStr">
-        <is>
-          <t>david@email.com</t>
-        </is>
-      </c>
-      <c r="W6" t="inlineStr">
-        <is>
           <t>Dinner</t>
         </is>
       </c>
+      <c r="V6" t="n">
+        <v>10</v>
+      </c>
+      <c r="W6" t="n">
+        <v>0.6</v>
+      </c>
       <c r="X6" t="n">
-        <v>10</v>
-      </c>
-      <c r="Y6" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="Z6" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1142,66 +1082,56 @@
           <t>S006</t>
         </is>
       </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>Spaghetti</t>
-        </is>
-      </c>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>Dinner</t>
-        </is>
-      </c>
-      <c r="M7" s="2" t="n">
+      <c r="K7" s="2" t="n">
         <v>45629.77083333334</v>
       </c>
-      <c r="N7" s="2" t="n">
+      <c r="L7" s="2" t="n">
         <v>45629.79166666666</v>
       </c>
-      <c r="O7" t="n">
+      <c r="M7" t="n">
         <v>30</v>
       </c>
+      <c r="N7" t="n">
+        <v>4.3</v>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>Bob Smith</t>
+        </is>
+      </c>
       <c r="P7" t="n">
-        <v>4.3</v>
+        <v>35</v>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>Bob Smith</t>
-        </is>
-      </c>
-      <c r="R7" t="n">
-        <v>35</v>
+          <t>Los Angeles</t>
+        </is>
+      </c>
+      <c r="R7" s="2" t="n">
+        <v>44977</v>
       </c>
       <c r="S7" t="inlineStr">
         <is>
-          <t>Los Angeles</t>
-        </is>
-      </c>
-      <c r="T7" s="2" t="n">
-        <v>44977</v>
+          <t>987-654-3210</t>
+        </is>
+      </c>
+      <c r="T7" t="inlineStr">
+        <is>
+          <t>bob@email.com</t>
+        </is>
       </c>
       <c r="U7" t="inlineStr">
         <is>
-          <t>987-654-3210</t>
-        </is>
-      </c>
-      <c r="V7" t="inlineStr">
-        <is>
-          <t>bob@email.com</t>
-        </is>
-      </c>
-      <c r="W7" t="inlineStr">
-        <is>
           <t>Lunch</t>
         </is>
       </c>
+      <c r="V7" t="n">
+        <v>8</v>
+      </c>
+      <c r="W7" t="n">
+        <v>0.4666666666666667</v>
+      </c>
       <c r="X7" t="n">
-        <v>8</v>
-      </c>
-      <c r="Y7" t="n">
-        <v>0.4666666666666667</v>
-      </c>
-      <c r="Z7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1248,66 +1178,56 @@
           <t>S007</t>
         </is>
       </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>Grilled Chicken</t>
-        </is>
-      </c>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t>Dinner</t>
-        </is>
-      </c>
-      <c r="M8" s="2" t="n">
+      <c r="K8" s="2" t="n">
         <v>45630.75</v>
       </c>
-      <c r="N8" s="2" t="n">
+      <c r="L8" s="2" t="n">
         <v>45630.78125</v>
       </c>
-      <c r="O8" t="n">
+      <c r="M8" t="n">
         <v>45</v>
       </c>
+      <c r="N8" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>Emma White</t>
+        </is>
+      </c>
       <c r="P8" t="n">
-        <v>4.6</v>
+        <v>30</v>
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>Emma White</t>
-        </is>
-      </c>
-      <c r="R8" t="n">
-        <v>30</v>
+          <t>Seattle</t>
+        </is>
+      </c>
+      <c r="R8" s="2" t="n">
+        <v>45068</v>
       </c>
       <c r="S8" t="inlineStr">
         <is>
-          <t>Seattle</t>
-        </is>
-      </c>
-      <c r="T8" s="2" t="n">
-        <v>45068</v>
+          <t>777-888-9999</t>
+        </is>
+      </c>
+      <c r="T8" t="inlineStr">
+        <is>
+          <t>emma@email.com</t>
+        </is>
       </c>
       <c r="U8" t="inlineStr">
         <is>
-          <t>777-888-9999</t>
-        </is>
-      </c>
-      <c r="V8" t="inlineStr">
-        <is>
-          <t>emma@email.com</t>
-        </is>
-      </c>
-      <c r="W8" t="inlineStr">
-        <is>
           <t>Lunch</t>
         </is>
       </c>
+      <c r="V8" t="n">
+        <v>9</v>
+      </c>
+      <c r="W8" t="n">
+        <v>0.3</v>
+      </c>
       <c r="X8" t="n">
-        <v>9</v>
-      </c>
-      <c r="Y8" t="n">
-        <v>0.3</v>
-      </c>
-      <c r="Z8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1354,66 +1274,56 @@
           <t>S008</t>
         </is>
       </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>Veggie Burger</t>
-        </is>
-      </c>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>Lunch</t>
-        </is>
-      </c>
-      <c r="M9" s="2" t="n">
+      <c r="K9" s="2" t="n">
         <v>45630.5625</v>
       </c>
-      <c r="N9" s="2" t="n">
+      <c r="L9" s="2" t="n">
         <v>45630.57638888889</v>
       </c>
-      <c r="O9" t="n">
+      <c r="M9" t="n">
         <v>20</v>
       </c>
+      <c r="N9" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>Charlie Lee</t>
+        </is>
+      </c>
       <c r="P9" t="n">
-        <v>4.4</v>
+        <v>42</v>
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>Charlie Lee</t>
-        </is>
-      </c>
-      <c r="R9" t="n">
-        <v>42</v>
+          <t>Chicago</t>
+        </is>
+      </c>
+      <c r="R9" s="2" t="n">
+        <v>44995</v>
       </c>
       <c r="S9" t="inlineStr">
         <is>
-          <t>Chicago</t>
-        </is>
-      </c>
-      <c r="T9" s="2" t="n">
-        <v>44995</v>
+          <t>555-123-4567</t>
+        </is>
+      </c>
+      <c r="T9" t="inlineStr">
+        <is>
+          <t>charlie@email.com</t>
+        </is>
       </c>
       <c r="U9" t="inlineStr">
         <is>
-          <t>555-123-4567</t>
-        </is>
-      </c>
-      <c r="V9" t="inlineStr">
-        <is>
-          <t>charlie@email.com</t>
-        </is>
-      </c>
-      <c r="W9" t="inlineStr">
-        <is>
           <t>Breakfast</t>
         </is>
       </c>
+      <c r="V9" t="n">
+        <v>15</v>
+      </c>
+      <c r="W9" t="n">
+        <v>0.55</v>
+      </c>
       <c r="X9" t="n">
-        <v>15</v>
-      </c>
-      <c r="Y9" t="n">
-        <v>0.55</v>
-      </c>
-      <c r="Z9" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1460,66 +1370,56 @@
           <t>S009</t>
         </is>
       </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>Grilled Chicken</t>
-        </is>
-      </c>
-      <c r="L10" t="inlineStr">
+      <c r="K10" s="2" t="n">
+        <v>45631.79166666666</v>
+      </c>
+      <c r="L10" s="2" t="n">
+        <v>45631.81944444445</v>
+      </c>
+      <c r="M10" t="n">
+        <v>40</v>
+      </c>
+      <c r="N10" t="n">
+        <v>4.9</v>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>Alice Johnson</t>
+        </is>
+      </c>
+      <c r="P10" t="n">
+        <v>28</v>
+      </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>New York</t>
+        </is>
+      </c>
+      <c r="R10" s="2" t="n">
+        <v>44941</v>
+      </c>
+      <c r="S10" t="inlineStr">
+        <is>
+          <t>123-456-7890</t>
+        </is>
+      </c>
+      <c r="T10" t="inlineStr">
+        <is>
+          <t>alice@email.com</t>
+        </is>
+      </c>
+      <c r="U10" t="inlineStr">
         <is>
           <t>Dinner</t>
         </is>
       </c>
-      <c r="M10" s="2" t="n">
-        <v>45631.79166666666</v>
-      </c>
-      <c r="N10" s="2" t="n">
-        <v>45631.81944444445</v>
-      </c>
-      <c r="O10" t="n">
-        <v>40</v>
-      </c>
-      <c r="P10" t="n">
-        <v>4.9</v>
-      </c>
-      <c r="Q10" t="inlineStr">
-        <is>
-          <t>Alice Johnson</t>
-        </is>
-      </c>
-      <c r="R10" t="n">
-        <v>28</v>
-      </c>
-      <c r="S10" t="inlineStr">
-        <is>
-          <t>New York</t>
-        </is>
-      </c>
-      <c r="T10" s="2" t="n">
-        <v>44941</v>
-      </c>
-      <c r="U10" t="inlineStr">
-        <is>
-          <t>123-456-7890</t>
-        </is>
-      </c>
-      <c r="V10" t="inlineStr">
-        <is>
-          <t>alice@email.com</t>
-        </is>
-      </c>
-      <c r="W10" t="inlineStr">
-        <is>
-          <t>Dinner</t>
-        </is>
+      <c r="V10" t="n">
+        <v>12</v>
+      </c>
+      <c r="W10" t="n">
+        <v>0.3</v>
       </c>
       <c r="X10" t="n">
-        <v>12</v>
-      </c>
-      <c r="Y10" t="n">
-        <v>0.3</v>
-      </c>
-      <c r="Z10" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1566,66 +1466,56 @@
           <t>S010</t>
         </is>
       </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>Oatmeal</t>
-        </is>
-      </c>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>Breakfast</t>
-        </is>
-      </c>
-      <c r="M11" s="2" t="n">
+      <c r="K11" s="2" t="n">
         <v>45631.29166666666</v>
       </c>
-      <c r="N11" s="2" t="n">
+      <c r="L11" s="2" t="n">
         <v>45631.29861111111</v>
       </c>
-      <c r="O11" t="n">
+      <c r="M11" t="n">
         <v>10</v>
       </c>
+      <c r="N11" t="n">
+        <v>4.1</v>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>Bob Smith</t>
+        </is>
+      </c>
       <c r="P11" t="n">
-        <v>4.1</v>
+        <v>35</v>
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>Bob Smith</t>
-        </is>
-      </c>
-      <c r="R11" t="n">
-        <v>35</v>
+          <t>Los Angeles</t>
+        </is>
+      </c>
+      <c r="R11" s="2" t="n">
+        <v>44977</v>
       </c>
       <c r="S11" t="inlineStr">
         <is>
-          <t>Los Angeles</t>
-        </is>
-      </c>
-      <c r="T11" s="2" t="n">
-        <v>44977</v>
+          <t>987-654-3210</t>
+        </is>
+      </c>
+      <c r="T11" t="inlineStr">
+        <is>
+          <t>bob@email.com</t>
+        </is>
       </c>
       <c r="U11" t="inlineStr">
         <is>
-          <t>987-654-3210</t>
-        </is>
-      </c>
-      <c r="V11" t="inlineStr">
-        <is>
-          <t>bob@email.com</t>
-        </is>
-      </c>
-      <c r="W11" t="inlineStr">
-        <is>
           <t>Lunch</t>
         </is>
       </c>
+      <c r="V11" t="n">
+        <v>8</v>
+      </c>
+      <c r="W11" t="n">
+        <v>0.7</v>
+      </c>
       <c r="X11" t="n">
-        <v>8</v>
-      </c>
-      <c r="Y11" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="Z11" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1672,66 +1562,56 @@
           <t>S011</t>
         </is>
       </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>Pancakes</t>
-        </is>
-      </c>
-      <c r="L12" t="inlineStr">
+      <c r="K12" s="2" t="n">
+        <v>45632.33333333334</v>
+      </c>
+      <c r="L12" s="2" t="n">
+        <v>45632.35416666666</v>
+      </c>
+      <c r="M12" t="n">
+        <v>30</v>
+      </c>
+      <c r="N12" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>Charlie Lee</t>
+        </is>
+      </c>
+      <c r="P12" t="n">
+        <v>42</v>
+      </c>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>Chicago</t>
+        </is>
+      </c>
+      <c r="R12" s="2" t="n">
+        <v>44995</v>
+      </c>
+      <c r="S12" t="inlineStr">
+        <is>
+          <t>555-123-4567</t>
+        </is>
+      </c>
+      <c r="T12" t="inlineStr">
+        <is>
+          <t>charlie@email.com</t>
+        </is>
+      </c>
+      <c r="U12" t="inlineStr">
         <is>
           <t>Breakfast</t>
         </is>
       </c>
-      <c r="M12" s="2" t="n">
-        <v>45632.33333333334</v>
-      </c>
-      <c r="N12" s="2" t="n">
-        <v>45632.35416666666</v>
-      </c>
-      <c r="O12" t="n">
-        <v>30</v>
-      </c>
-      <c r="P12" t="n">
-        <v>4.6</v>
-      </c>
-      <c r="Q12" t="inlineStr">
-        <is>
-          <t>Charlie Lee</t>
-        </is>
-      </c>
-      <c r="R12" t="n">
-        <v>42</v>
-      </c>
-      <c r="S12" t="inlineStr">
-        <is>
-          <t>Chicago</t>
-        </is>
-      </c>
-      <c r="T12" s="2" t="n">
-        <v>44995</v>
-      </c>
-      <c r="U12" t="inlineStr">
-        <is>
-          <t>555-123-4567</t>
-        </is>
-      </c>
-      <c r="V12" t="inlineStr">
-        <is>
-          <t>charlie@email.com</t>
-        </is>
-      </c>
-      <c r="W12" t="inlineStr">
-        <is>
-          <t>Breakfast</t>
-        </is>
+      <c r="V12" t="n">
+        <v>15</v>
+      </c>
+      <c r="W12" t="n">
+        <v>0.2833333333333333</v>
       </c>
       <c r="X12" t="n">
-        <v>15</v>
-      </c>
-      <c r="Y12" t="n">
-        <v>0.2833333333333333</v>
-      </c>
-      <c r="Z12" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1778,66 +1658,56 @@
           <t>S012</t>
         </is>
       </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>Spaghetti</t>
-        </is>
-      </c>
-      <c r="L13" t="inlineStr">
+      <c r="K13" s="2" t="n">
+        <v>45632.79166666666</v>
+      </c>
+      <c r="L13" s="2" t="n">
+        <v>45632.81944444445</v>
+      </c>
+      <c r="M13" t="n">
+        <v>40</v>
+      </c>
+      <c r="N13" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>David Brown</t>
+        </is>
+      </c>
+      <c r="P13" t="n">
+        <v>27</v>
+      </c>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>San Francisco</t>
+        </is>
+      </c>
+      <c r="R13" s="2" t="n">
+        <v>45021</v>
+      </c>
+      <c r="S13" t="inlineStr">
+        <is>
+          <t>444-333-2222</t>
+        </is>
+      </c>
+      <c r="T13" t="inlineStr">
+        <is>
+          <t>david@email.com</t>
+        </is>
+      </c>
+      <c r="U13" t="inlineStr">
         <is>
           <t>Dinner</t>
         </is>
       </c>
-      <c r="M13" s="2" t="n">
-        <v>45632.79166666666</v>
-      </c>
-      <c r="N13" s="2" t="n">
-        <v>45632.81944444445</v>
-      </c>
-      <c r="O13" t="n">
-        <v>40</v>
-      </c>
-      <c r="P13" t="n">
-        <v>4.7</v>
-      </c>
-      <c r="Q13" t="inlineStr">
-        <is>
-          <t>David Brown</t>
-        </is>
-      </c>
-      <c r="R13" t="n">
-        <v>27</v>
-      </c>
-      <c r="S13" t="inlineStr">
-        <is>
-          <t>San Francisco</t>
-        </is>
-      </c>
-      <c r="T13" s="2" t="n">
-        <v>45021</v>
-      </c>
-      <c r="U13" t="inlineStr">
-        <is>
-          <t>444-333-2222</t>
-        </is>
-      </c>
-      <c r="V13" t="inlineStr">
-        <is>
-          <t>david@email.com</t>
-        </is>
-      </c>
-      <c r="W13" t="inlineStr">
-        <is>
-          <t>Dinner</t>
-        </is>
+      <c r="V13" t="n">
+        <v>10</v>
+      </c>
+      <c r="W13" t="n">
+        <v>0.3125</v>
       </c>
       <c r="X13" t="n">
-        <v>10</v>
-      </c>
-      <c r="Y13" t="n">
-        <v>0.3125</v>
-      </c>
-      <c r="Z13" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1884,66 +1754,56 @@
           <t>S013</t>
         </is>
       </c>
-      <c r="K14" t="inlineStr">
-        <is>
-          <t>Caesar Salad</t>
-        </is>
-      </c>
-      <c r="L14" t="inlineStr">
+      <c r="K14" s="2" t="n">
+        <v>45633.52083333334</v>
+      </c>
+      <c r="L14" s="2" t="n">
+        <v>45633.54166666666</v>
+      </c>
+      <c r="M14" t="n">
+        <v>30</v>
+      </c>
+      <c r="N14" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>Emma White</t>
+        </is>
+      </c>
+      <c r="P14" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q14" t="inlineStr">
+        <is>
+          <t>Seattle</t>
+        </is>
+      </c>
+      <c r="R14" s="2" t="n">
+        <v>45068</v>
+      </c>
+      <c r="S14" t="inlineStr">
+        <is>
+          <t>777-888-9999</t>
+        </is>
+      </c>
+      <c r="T14" t="inlineStr">
+        <is>
+          <t>emma@email.com</t>
+        </is>
+      </c>
+      <c r="U14" t="inlineStr">
         <is>
           <t>Lunch</t>
         </is>
       </c>
-      <c r="M14" s="2" t="n">
-        <v>45633.52083333334</v>
-      </c>
-      <c r="N14" s="2" t="n">
-        <v>45633.54166666666</v>
-      </c>
-      <c r="O14" t="n">
-        <v>30</v>
-      </c>
-      <c r="P14" t="n">
-        <v>4.4</v>
-      </c>
-      <c r="Q14" t="inlineStr">
-        <is>
-          <t>Emma White</t>
-        </is>
-      </c>
-      <c r="R14" t="n">
-        <v>30</v>
-      </c>
-      <c r="S14" t="inlineStr">
-        <is>
-          <t>Seattle</t>
-        </is>
-      </c>
-      <c r="T14" s="2" t="n">
-        <v>45068</v>
-      </c>
-      <c r="U14" t="inlineStr">
-        <is>
-          <t>777-888-9999</t>
-        </is>
-      </c>
-      <c r="V14" t="inlineStr">
-        <is>
-          <t>emma@email.com</t>
-        </is>
-      </c>
-      <c r="W14" t="inlineStr">
-        <is>
-          <t>Lunch</t>
-        </is>
+      <c r="V14" t="n">
+        <v>9</v>
+      </c>
+      <c r="W14" t="n">
+        <v>0.3</v>
       </c>
       <c r="X14" t="n">
-        <v>9</v>
-      </c>
-      <c r="Y14" t="n">
-        <v>0.3</v>
-      </c>
-      <c r="Z14" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1990,66 +1850,56 @@
           <t>S014</t>
         </is>
       </c>
-      <c r="K15" t="inlineStr">
-        <is>
-          <t>Grilled Chicken</t>
-        </is>
-      </c>
-      <c r="L15" t="inlineStr">
+      <c r="K15" s="2" t="n">
+        <v>45633.75</v>
+      </c>
+      <c r="L15" s="2" t="n">
+        <v>45633.78125</v>
+      </c>
+      <c r="M15" t="n">
+        <v>45</v>
+      </c>
+      <c r="N15" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>Frank Green</t>
+        </is>
+      </c>
+      <c r="P15" t="n">
+        <v>25</v>
+      </c>
+      <c r="Q15" t="inlineStr">
+        <is>
+          <t>Austin</t>
+        </is>
+      </c>
+      <c r="R15" s="2" t="n">
+        <v>45092</v>
+      </c>
+      <c r="S15" t="inlineStr">
+        <is>
+          <t>888-777-6666</t>
+        </is>
+      </c>
+      <c r="T15" t="inlineStr">
+        <is>
+          <t>frank@email.com</t>
+        </is>
+      </c>
+      <c r="U15" t="inlineStr">
         <is>
           <t>Dinner</t>
         </is>
       </c>
-      <c r="M15" s="2" t="n">
-        <v>45633.75</v>
-      </c>
-      <c r="N15" s="2" t="n">
-        <v>45633.78125</v>
-      </c>
-      <c r="O15" t="n">
-        <v>45</v>
-      </c>
-      <c r="P15" t="n">
-        <v>4.8</v>
-      </c>
-      <c r="Q15" t="inlineStr">
-        <is>
-          <t>Frank Green</t>
-        </is>
-      </c>
-      <c r="R15" t="n">
-        <v>25</v>
-      </c>
-      <c r="S15" t="inlineStr">
-        <is>
-          <t>Austin</t>
-        </is>
-      </c>
-      <c r="T15" s="2" t="n">
-        <v>45092</v>
-      </c>
-      <c r="U15" t="inlineStr">
-        <is>
-          <t>888-777-6666</t>
-        </is>
-      </c>
-      <c r="V15" t="inlineStr">
-        <is>
-          <t>frank@email.com</t>
-        </is>
-      </c>
-      <c r="W15" t="inlineStr">
-        <is>
-          <t>Dinner</t>
-        </is>
+      <c r="V15" t="n">
+        <v>7</v>
+      </c>
+      <c r="W15" t="n">
+        <v>0.2888888888888889</v>
       </c>
       <c r="X15" t="n">
-        <v>7</v>
-      </c>
-      <c r="Y15" t="n">
-        <v>0.2888888888888889</v>
-      </c>
-      <c r="Z15" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2096,66 +1946,56 @@
           <t>S015</t>
         </is>
       </c>
-      <c r="K16" t="inlineStr">
-        <is>
-          <t>Spaghetti</t>
-        </is>
-      </c>
-      <c r="L16" t="inlineStr">
-        <is>
-          <t>Dinner</t>
-        </is>
-      </c>
-      <c r="M16" s="2" t="n">
+      <c r="K16" s="2" t="n">
         <v>45634.8125</v>
       </c>
-      <c r="N16" s="2" t="n">
+      <c r="L16" s="2" t="n">
         <v>45634.84027777778</v>
       </c>
-      <c r="O16" t="n">
+      <c r="M16" t="n">
         <v>40</v>
       </c>
+      <c r="N16" t="n">
+        <v>5</v>
+      </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>Grace King</t>
+        </is>
+      </c>
       <c r="P16" t="n">
-        <v>5</v>
+        <v>38</v>
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>Grace King</t>
-        </is>
-      </c>
-      <c r="R16" t="n">
-        <v>38</v>
+          <t>Boston</t>
+        </is>
+      </c>
+      <c r="R16" s="2" t="n">
+        <v>45109</v>
       </c>
       <c r="S16" t="inlineStr">
         <is>
-          <t>Boston</t>
-        </is>
-      </c>
-      <c r="T16" s="2" t="n">
-        <v>45109</v>
+          <t>999-888-7777</t>
+        </is>
+      </c>
+      <c r="T16" t="inlineStr">
+        <is>
+          <t>grace@email.com</t>
+        </is>
       </c>
       <c r="U16" t="inlineStr">
         <is>
-          <t>999-888-7777</t>
-        </is>
-      </c>
-      <c r="V16" t="inlineStr">
-        <is>
-          <t>grace@email.com</t>
-        </is>
-      </c>
-      <c r="W16" t="inlineStr">
-        <is>
           <t>Breakfast</t>
         </is>
       </c>
+      <c r="V16" t="n">
+        <v>14</v>
+      </c>
+      <c r="W16" t="n">
+        <v>0.35</v>
+      </c>
       <c r="X16" t="n">
-        <v>14</v>
-      </c>
-      <c r="Y16" t="n">
-        <v>0.35</v>
-      </c>
-      <c r="Z16" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2202,66 +2042,56 @@
           <t>S016</t>
         </is>
       </c>
-      <c r="K17" t="inlineStr">
-        <is>
-          <t>Veggie Burger</t>
-        </is>
-      </c>
-      <c r="L17" t="inlineStr">
-        <is>
-          <t>Lunch</t>
-        </is>
-      </c>
-      <c r="M17" s="2" t="n">
+      <c r="K17" s="2" t="n">
         <v>45634.5625</v>
       </c>
-      <c r="N17" s="2" t="n">
+      <c r="L17" s="2" t="n">
         <v>45634.57638888889</v>
       </c>
-      <c r="O17" t="n">
+      <c r="M17" t="n">
         <v>20</v>
       </c>
+      <c r="N17" t="n">
+        <v>4.3</v>
+      </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>Henry Lee</t>
+        </is>
+      </c>
       <c r="P17" t="n">
-        <v>4.3</v>
+        <v>31</v>
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>Henry Lee</t>
-        </is>
-      </c>
-      <c r="R17" t="n">
-        <v>31</v>
+          <t>Miami</t>
+        </is>
+      </c>
+      <c r="R17" s="2" t="n">
+        <v>45149</v>
       </c>
       <c r="S17" t="inlineStr">
         <is>
-          <t>Miami</t>
-        </is>
-      </c>
-      <c r="T17" s="2" t="n">
-        <v>45149</v>
+          <t>101-202-3030</t>
+        </is>
+      </c>
+      <c r="T17" t="inlineStr">
+        <is>
+          <t>henry@email.com</t>
+        </is>
       </c>
       <c r="U17" t="inlineStr">
         <is>
-          <t>101-202-3030</t>
-        </is>
-      </c>
-      <c r="V17" t="inlineStr">
-        <is>
-          <t>henry@email.com</t>
-        </is>
-      </c>
-      <c r="W17" t="inlineStr">
-        <is>
           <t>Dinner</t>
         </is>
       </c>
+      <c r="V17" t="n">
+        <v>5</v>
+      </c>
+      <c r="W17" t="n">
+        <v>0.55</v>
+      </c>
       <c r="X17" t="n">
-        <v>5</v>
-      </c>
-      <c r="Y17" t="n">
-        <v>0.55</v>
-      </c>
-      <c r="Z17" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>